<commit_message>
Fix H_GovernmentResponseIndexForDisplay_norm in indicator agg
The `Indicator aggregation.xlsx` sheet previously listed
`H_GovernmentResponseIndexForDisplay` on the `Emerging Risk` sheet. The id in
the `Indicator Label` sheet is `H_GovernmentResponseIndexForDisplay_norm`. In
this commit we update the `Emerging Risk` sheet to use
`GovernmentResponseIndexForDisplay_norm`.
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="227">
   <si>
     <t xml:space="preserve">INDICATOR NAME</t>
   </si>
@@ -560,7 +560,7 @@
 0 &lt;= 0 </t>
   </si>
   <si>
-    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay</t>
+    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay_norm</t>
   </si>
   <si>
     <t xml:space="preserve">Oxford Government Response Index (Oxford University - Blavatnik)</t>
@@ -1631,9 +1631,6 @@
   </si>
   <si>
     <t xml:space="preserve">Covid Growth, Deaths (biweekly)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay_norm</t>
   </si>
   <si>
     <t xml:space="preserve">Oxford Gov Response Index</t>
@@ -2239,7 +2236,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2710,10 +2707,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="17" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="25" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2900,9 +2893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2847240</xdr:colOff>
+      <xdr:colOff>2846880</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>487440</xdr:rowOff>
+      <xdr:rowOff>487080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2916,7 +2909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17074080" y="5455080"/>
-          <a:ext cx="710640" cy="226440"/>
+          <a:ext cx="710280" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2937,9 +2930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2768040</xdr:colOff>
+      <xdr:colOff>2767680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>879120</xdr:rowOff>
+      <xdr:rowOff>878760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2953,7 +2946,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16931520" y="5846760"/>
-          <a:ext cx="774000" cy="226440"/>
+          <a:ext cx="773640" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2974,9 +2967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>261360</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1270800</xdr:rowOff>
+      <xdr:rowOff>1270440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2990,7 +2983,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17014680" y="6238440"/>
-          <a:ext cx="1550880" cy="226440"/>
+          <a:ext cx="1550520" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3011,9 +3004,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2598840</xdr:colOff>
+      <xdr:colOff>2598480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1710000</xdr:rowOff>
+      <xdr:rowOff>1709640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3027,7 +3020,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16990920" y="6677640"/>
-          <a:ext cx="545400" cy="226440"/>
+          <a:ext cx="545040" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3048,9 +3041,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2786040</xdr:colOff>
+      <xdr:colOff>2785680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2102400</xdr:rowOff>
+      <xdr:rowOff>2102040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3064,7 +3057,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17038440" y="7057440"/>
-          <a:ext cx="685080" cy="239040"/>
+          <a:ext cx="684720" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3085,9 +3078,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2735280</xdr:colOff>
+      <xdr:colOff>2734920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2505960</xdr:rowOff>
+      <xdr:rowOff>2505600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3101,7 +3094,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17038440" y="7461000"/>
-          <a:ext cx="634320" cy="239040"/>
+          <a:ext cx="633960" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3122,9 +3115,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3116160</xdr:colOff>
+      <xdr:colOff>3115800</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2921400</xdr:rowOff>
+      <xdr:rowOff>2921040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3138,7 +3131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17418240" y="7876440"/>
-          <a:ext cx="635400" cy="239040"/>
+          <a:ext cx="635040" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3165,11 +3158,11 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="36.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="62.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="43.5"/>
   </cols>
@@ -3437,8 +3430,8 @@
   </sheetPr>
   <dimension ref="A1:CP34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5784,7 +5777,7 @@
       <c r="CO24" s="60"/>
       <c r="CP24" s="60"/>
     </row>
-    <row r="25" s="83" customFormat="true" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="83" customFormat="true" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="92" t="s">
         <v>96</v>
       </c>
@@ -6750,12 +6743,12 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="101" width="35.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="101" width="35.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6996,10 +6989,10 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.828125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7142,12 +7135,12 @@
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="108" width="146.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.33"/>
   </cols>
@@ -7294,7 +7287,7 @@
       <c r="C9" s="117" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="113" t="s">
         <v>198</v>
       </c>
       <c r="E9" s="111" t="s">
@@ -7312,7 +7305,7 @@
       <c r="C10" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="113" t="s">
         <v>200</v>
       </c>
       <c r="E10" s="111"/>
@@ -7325,7 +7318,7 @@
       <c r="B11" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="118" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="107" t="s">
@@ -7341,7 +7334,7 @@
       <c r="B12" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="118" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="107" t="s">
@@ -7359,7 +7352,7 @@
       <c r="B13" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="119" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="107" t="s">
@@ -7375,7 +7368,7 @@
       <c r="B14" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="119" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="107" t="s">
@@ -7391,7 +7384,7 @@
       <c r="B15" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="120" t="s">
+      <c r="C15" s="119" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="107" t="s">
@@ -7409,7 +7402,7 @@
       <c r="B16" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="120" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="107" t="s">
@@ -7425,7 +7418,7 @@
       <c r="B17" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="120" t="s">
         <v>209</v>
       </c>
       <c r="D17" s="107" t="s">
@@ -7441,7 +7434,7 @@
       <c r="B18" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="121" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="107" t="s">
@@ -7457,7 +7450,7 @@
       <c r="B19" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="121" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="107" t="s">
@@ -7473,7 +7466,7 @@
       <c r="B20" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="121" t="s">
         <v>213</v>
       </c>
       <c r="D20" s="113" t="s">
@@ -7489,7 +7482,7 @@
       <c r="B21" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="121" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="113" t="s">
@@ -7505,7 +7498,7 @@
       <c r="B22" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="121" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="113" t="s">
@@ -7521,7 +7514,7 @@
       <c r="B23" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="122" t="s">
         <v>83</v>
       </c>
       <c r="D23" s="107" t="s">
@@ -7537,7 +7530,7 @@
       <c r="B24" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="122" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="107" t="s">
@@ -7553,11 +7546,11 @@
       <c r="B25" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="107" t="s">
         <v>219</v>
-      </c>
-      <c r="D25" s="107" t="s">
-        <v>220</v>
       </c>
       <c r="E25" s="111"/>
       <c r="F25" s="107"/>
@@ -7569,11 +7562,11 @@
       <c r="B26" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="123" t="s">
+      <c r="C26" s="122" t="s">
         <v>102</v>
       </c>
       <c r="D26" s="107" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E26" s="111"/>
       <c r="F26" s="107"/>
@@ -7585,11 +7578,11 @@
       <c r="B27" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="123" t="s">
+      <c r="C27" s="122" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E27" s="111"/>
     </row>
@@ -7600,11 +7593,11 @@
       <c r="B28" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="123" t="s">
+      <c r="C28" s="122" t="s">
         <v>93</v>
       </c>
       <c r="D28" s="107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E28" s="111"/>
     </row>
@@ -7615,11 +7608,11 @@
       <c r="B29" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="123" t="s">
+      <c r="C29" s="122" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E29" s="111"/>
     </row>
@@ -7630,11 +7623,11 @@
       <c r="B30" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="122" t="s">
         <v>99</v>
       </c>
       <c r="D30" s="107" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E30" s="111"/>
     </row>
@@ -7645,7 +7638,7 @@
       <c r="B31" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="123" t="s">
         <v>116</v>
       </c>
       <c r="D31" s="107" t="s">
@@ -7660,11 +7653,11 @@
       <c r="B32" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="123" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="107" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E32" s="111"/>
     </row>
@@ -7675,7 +7668,7 @@
       <c r="B33" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="123" t="s">
         <v>108</v>
       </c>
       <c r="D33" s="107" t="s">
@@ -7691,31 +7684,31 @@
       <c r="B34" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="123" t="s">
         <v>111</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="E34" s="125"/>
+        <v>226</v>
+      </c>
+      <c r="E34" s="124"/>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="125"/>
+      <c r="E35" s="124"/>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="125"/>
+      <c r="E36" s="124"/>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="125"/>
+      <c r="E37" s="124"/>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="125"/>
+      <c r="E38" s="124"/>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="125"/>
+      <c r="E39" s="124"/>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="125"/>
+      <c r="E40" s="124"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D20:D25 D2:D17 D29:D33">

</xml_diff>

<commit_message>
Update emerging indicator names in Indicator aggregation
When running the build we saw the following warnings in the console

WARNING: Indicator 'S_income_support.Rating_norm' in category 'socioeconomic'
does not have a display name
WARNING: Indicator 'H_GovernmentResponseIndexForDisplay' in category 'health'
does not have a display name

We edit the first column in the Emerging Risk tab of Indicator aggregation so
that the indicator names match

S_income_support.Rating_norm
to
S_income_support.Rating_crm_norm

H_GovernmentResponseIndexForDisplay
to
H_GovernmentResponseIndexForDisplay_norm
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="226">
   <si>
     <t xml:space="preserve">INDICATOR NAME</t>
   </si>
@@ -467,7 +467,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">S_income_support.Rating_norm</t>
+    <t xml:space="preserve">S_income_support.Rating_crm_norm</t>
   </si>
   <si>
     <t xml:space="preserve">Whether income support is provided</t>
@@ -560,7 +560,7 @@
 0 &lt;= 0 </t>
   </si>
   <si>
-    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay</t>
+    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay_norm</t>
   </si>
   <si>
     <t xml:space="preserve">Oxford Government Response Index (Oxford University - Blavatnik)</t>
@@ -1615,9 +1615,6 @@
     <t xml:space="preserve">MFRI Household Level Risk</t>
   </si>
   <si>
-    <t xml:space="preserve">S_income_support.Rating_crm_norm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Income Support</t>
   </si>
   <si>
@@ -1631,9 +1628,6 @@
   </si>
   <si>
     <t xml:space="preserve">Covid Growth, Deaths (biweekly)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H_GovernmentResponseIndexForDisplay_norm</t>
   </si>
   <si>
     <t xml:space="preserve">Oxford Gov Response Index</t>
@@ -2239,7 +2233,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2710,10 +2704,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="17" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="25" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2900,9 +2890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2847240</xdr:colOff>
+      <xdr:colOff>2846880</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>487440</xdr:rowOff>
+      <xdr:rowOff>487080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2916,7 +2906,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17074080" y="5455080"/>
-          <a:ext cx="710640" cy="226440"/>
+          <a:ext cx="710280" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2937,9 +2927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2768040</xdr:colOff>
+      <xdr:colOff>2767680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>879120</xdr:rowOff>
+      <xdr:rowOff>878760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2953,7 +2943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16931520" y="5846760"/>
-          <a:ext cx="774000" cy="226440"/>
+          <a:ext cx="773640" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2974,9 +2964,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>261360</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1270800</xdr:rowOff>
+      <xdr:rowOff>1270440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2990,7 +2980,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17014680" y="6238440"/>
-          <a:ext cx="1550880" cy="226440"/>
+          <a:ext cx="1550520" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3011,9 +3001,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2598840</xdr:colOff>
+      <xdr:colOff>2598480</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1710000</xdr:rowOff>
+      <xdr:rowOff>1709640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3027,7 +3017,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16990920" y="6677640"/>
-          <a:ext cx="545400" cy="226440"/>
+          <a:ext cx="545040" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3048,9 +3038,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2786040</xdr:colOff>
+      <xdr:colOff>2785680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2102400</xdr:rowOff>
+      <xdr:rowOff>2102040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3064,7 +3054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17038440" y="7057440"/>
-          <a:ext cx="685080" cy="239040"/>
+          <a:ext cx="684720" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3085,9 +3075,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2735280</xdr:colOff>
+      <xdr:colOff>2734920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2505960</xdr:rowOff>
+      <xdr:rowOff>2505600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3101,7 +3091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17038440" y="7461000"/>
-          <a:ext cx="634320" cy="239040"/>
+          <a:ext cx="633960" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3122,9 +3112,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3116160</xdr:colOff>
+      <xdr:colOff>3115800</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2921400</xdr:rowOff>
+      <xdr:rowOff>2921040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3138,7 +3128,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17418240" y="7876440"/>
-          <a:ext cx="635400" cy="239040"/>
+          <a:ext cx="635040" cy="238680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3161,15 +3151,15 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="36.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="62.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="43.5"/>
   </cols>
@@ -3437,8 +3427,8 @@
   </sheetPr>
   <dimension ref="A1:CP34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5070,7 +5060,7 @@
       <c r="CO17" s="60"/>
       <c r="CP17" s="60"/>
     </row>
-    <row r="18" s="83" customFormat="true" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="83" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="88" t="s">
         <v>77</v>
       </c>
@@ -5784,7 +5774,7 @@
       <c r="CO24" s="60"/>
       <c r="CP24" s="60"/>
     </row>
-    <row r="25" s="83" customFormat="true" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="83" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="92" t="s">
         <v>96</v>
       </c>
@@ -6746,16 +6736,16 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="101" width="35.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="101" width="35.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6992,14 +6982,14 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.828125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7138,16 +7128,16 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C12" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="108" width="146.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.33"/>
   </cols>
@@ -7294,7 +7284,7 @@
       <c r="C9" s="117" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="113" t="s">
         <v>198</v>
       </c>
       <c r="E9" s="111" t="s">
@@ -7312,7 +7302,7 @@
       <c r="C10" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="113" t="s">
         <v>200</v>
       </c>
       <c r="E10" s="111"/>
@@ -7325,7 +7315,7 @@
       <c r="B11" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="118" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="107" t="s">
@@ -7341,7 +7331,7 @@
       <c r="B12" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="118" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="107" t="s">
@@ -7359,7 +7349,7 @@
       <c r="B13" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="119" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="107" t="s">
@@ -7375,7 +7365,7 @@
       <c r="B14" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="119" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="107" t="s">
@@ -7391,7 +7381,7 @@
       <c r="B15" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="120" t="s">
+      <c r="C15" s="119" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="107" t="s">
@@ -7409,7 +7399,7 @@
       <c r="B16" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="120" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="107" t="s">
@@ -7425,7 +7415,7 @@
       <c r="B17" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="120" t="s">
         <v>209</v>
       </c>
       <c r="D17" s="107" t="s">
@@ -7441,7 +7431,7 @@
       <c r="B18" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="121" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="107" t="s">
@@ -7457,7 +7447,7 @@
       <c r="B19" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="121" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="107" t="s">
@@ -7473,11 +7463,11 @@
       <c r="B20" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C20" s="121" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="113" t="s">
         <v>213</v>
-      </c>
-      <c r="D20" s="113" t="s">
-        <v>214</v>
       </c>
       <c r="E20" s="111"/>
       <c r="F20" s="107"/>
@@ -7489,11 +7479,11 @@
       <c r="B21" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="121" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="113" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21" s="111"/>
       <c r="F21" s="107"/>
@@ -7505,11 +7495,11 @@
       <c r="B22" s="107" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="122" t="s">
+      <c r="C22" s="121" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="113" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E22" s="111"/>
       <c r="F22" s="107"/>
@@ -7521,11 +7511,11 @@
       <c r="B23" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="122" t="s">
         <v>83</v>
       </c>
       <c r="D23" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E23" s="111"/>
       <c r="F23" s="107"/>
@@ -7537,11 +7527,11 @@
       <c r="B24" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="122" t="s">
         <v>87</v>
       </c>
       <c r="D24" s="107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24" s="111"/>
       <c r="F24" s="107"/>
@@ -7553,11 +7543,11 @@
       <c r="B25" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="123" t="s">
-        <v>219</v>
+      <c r="C25" s="122" t="s">
+        <v>96</v>
       </c>
       <c r="D25" s="107" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E25" s="111"/>
       <c r="F25" s="107"/>
@@ -7569,11 +7559,11 @@
       <c r="B26" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="123" t="s">
+      <c r="C26" s="122" t="s">
         <v>102</v>
       </c>
       <c r="D26" s="107" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E26" s="111"/>
       <c r="F26" s="107"/>
@@ -7585,11 +7575,11 @@
       <c r="B27" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="123" t="s">
+      <c r="C27" s="122" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="107" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E27" s="111"/>
     </row>
@@ -7600,11 +7590,11 @@
       <c r="B28" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="123" t="s">
+      <c r="C28" s="122" t="s">
         <v>93</v>
       </c>
       <c r="D28" s="107" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E28" s="111"/>
     </row>
@@ -7615,11 +7605,11 @@
       <c r="B29" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="123" t="s">
+      <c r="C29" s="122" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="107" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E29" s="111"/>
     </row>
@@ -7630,11 +7620,11 @@
       <c r="B30" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="122" t="s">
         <v>99</v>
       </c>
       <c r="D30" s="107" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E30" s="111"/>
     </row>
@@ -7645,7 +7635,7 @@
       <c r="B31" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="123" t="s">
         <v>116</v>
       </c>
       <c r="D31" s="107" t="s">
@@ -7660,11 +7650,11 @@
       <c r="B32" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="123" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="107" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E32" s="111"/>
     </row>
@@ -7675,7 +7665,7 @@
       <c r="B33" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="123" t="s">
         <v>108</v>
       </c>
       <c r="D33" s="107" t="s">
@@ -7691,31 +7681,31 @@
       <c r="B34" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="123" t="s">
         <v>111</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="E34" s="125"/>
+        <v>225</v>
+      </c>
+      <c r="E34" s="124"/>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="125"/>
+      <c r="E35" s="124"/>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="125"/>
+      <c r="E36" s="124"/>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="125"/>
+      <c r="E37" s="124"/>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="125"/>
+      <c r="E38" s="124"/>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="125"/>
+      <c r="E39" s="124"/>
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="125"/>
+      <c r="E40" s="124"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D20:D25 D2:D17 D29:D33">

</xml_diff>